<commit_message>
case with 380 kV done
</commit_message>
<xml_diff>
--- a/Code/Results/Cases/Case_0_0/diagnostic.xlsx
+++ b/Code/Results/Cases/Case_0_0/diagnostic.xlsx
@@ -13,29 +13,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>overload</t>
-  </si>
-  <si>
-    <t>wrong_switch_configuration</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -51,7 +32,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -59,30 +40,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,34 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
contingencies with rene fine
</commit_message>
<xml_diff>
--- a/Code/Results/Cases/Case_0_0/diagnostic.xlsx
+++ b/Code/Results/Cases/Case_0_0/diagnostic.xlsx
@@ -13,32 +13,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>disconnected_elements</t>
-  </si>
-  <si>
-    <t>overload</t>
-  </si>
-  <si>
-    <t>wrong_switch_configuration</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,7 +32,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -62,30 +40,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,42 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>